<commit_message>
Finished this version of the test plans. Yea!
</commit_message>
<xml_diff>
--- a/Testplans/Wallet Test Plan Suite.xlsx
+++ b/Testplans/Wallet Test Plan Suite.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="112">
   <si>
     <t>Agent 1</t>
   </si>
@@ -290,13 +290,79 @@
   </si>
   <si>
     <t>This test plan is exected in the testAgentWallets functional test</t>
+  </si>
+  <si>
+    <t>[ J I H F A ]</t>
+  </si>
+  <si>
+    <t>J10 Buys to I9</t>
+  </si>
+  <si>
+    <t>Buy / Sell - 5 Segment Path</t>
+  </si>
+  <si>
+    <t>I9 Receives from J10</t>
+  </si>
+  <si>
+    <t>Test 6</t>
+  </si>
+  <si>
+    <t>H9 Receives from I9</t>
+  </si>
+  <si>
+    <t>H8 Provies to F6</t>
+  </si>
+  <si>
+    <t>I9 Provies to H8</t>
+  </si>
+  <si>
+    <t>F6 Receives from H9</t>
+  </si>
+  <si>
+    <t>F6 Provies to A1</t>
+  </si>
+  <si>
+    <t>A1 Sells to F6</t>
+  </si>
+  <si>
+    <t>Tran 1</t>
+  </si>
+  <si>
+    <t>[ A F ]</t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>Tran 2</t>
+  </si>
+  <si>
+    <t>Test: Show that a longer path is selected if a shorter path is illiquid, in this case between A and B</t>
+  </si>
+  <si>
+    <t>Tran 3</t>
+  </si>
+  <si>
+    <t>[ A C D B ]</t>
+  </si>
+  <si>
+    <t>A3 Provides to D4</t>
+  </si>
+  <si>
+    <t>D4 Receives from C3</t>
+  </si>
+  <si>
+    <t>D4 Provides to B2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -360,6 +426,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3366FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -399,7 +471,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="108">
+  <cellStyleXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -508,8 +580,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -571,8 +667,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="108">
+  <cellStyles count="132">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -626,6 +725,18 @@
     <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -679,6 +790,18 @@
     <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1009,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O90"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1113,6 +1236,9 @@
       <c r="G8" s="11">
         <v>0.05</v>
       </c>
+      <c r="O8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="9" spans="1:15">
       <c r="C9" t="s">
@@ -1607,565 +1733,569 @@
       </c>
       <c r="N25" s="9"/>
     </row>
-    <row r="26" spans="1:14">
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+    <row r="26" spans="1:14" s="10" customFormat="1">
+      <c r="A26" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="14">
+        <f>E25+F26</f>
+        <v>628.75</v>
+      </c>
+      <c r="F26" s="5">
+        <v>125</v>
+      </c>
+      <c r="G26" s="5">
+        <v>6004</v>
+      </c>
+      <c r="H26" s="6">
+        <v>6</v>
+      </c>
+      <c r="I26" s="6">
+        <v>6</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L26" s="6">
+        <v>6</v>
+      </c>
+      <c r="M26" s="26">
+        <v>8</v>
+      </c>
+      <c r="N26" s="9"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="20" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B28" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20">
+      <c r="D28" s="20"/>
+      <c r="E28" s="20">
         <v>500</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F28" s="20">
         <v>500</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G28" s="20">
         <v>6001</v>
       </c>
-      <c r="H27" s="23">
+      <c r="H28" s="23">
         <v>2</v>
       </c>
-      <c r="I27" s="23">
-        <v>0</v>
-      </c>
-      <c r="J27" s="23">
+      <c r="I28" s="23">
+        <v>0</v>
+      </c>
+      <c r="J28" s="23">
         <v>2</v>
       </c>
-      <c r="K27" s="20" t="s">
+      <c r="K28" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L27" s="23">
-        <v>1</v>
-      </c>
-      <c r="M27" s="24">
-        <v>0</v>
-      </c>
-      <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="7" t="s">
+      <c r="L28" s="23">
+        <v>1</v>
+      </c>
+      <c r="M28" s="24">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="7">
-        <f>E27+F28</f>
-        <v>600</v>
-      </c>
-      <c r="F28" s="7">
-        <v>100</v>
-      </c>
-      <c r="G28" s="7">
-        <v>6004</v>
-      </c>
-      <c r="H28" s="8">
-        <v>1</v>
-      </c>
-      <c r="I28" s="8">
-        <v>1</v>
-      </c>
-      <c r="J28" s="8">
-        <v>2</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="L28" s="8">
-        <v>2</v>
-      </c>
-      <c r="M28" s="8">
-        <v>2</v>
-      </c>
-      <c r="N28" s="2"/>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="15">
+        <v>40</v>
+      </c>
+      <c r="E29" s="7">
         <f>E28+F29</f>
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="F29" s="7">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G29" s="7">
-        <v>6003</v>
+        <v>6004</v>
       </c>
       <c r="H29" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J29" s="8">
         <v>2</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="L29" s="8">
         <v>2</v>
       </c>
       <c r="M29" s="8">
+        <v>2</v>
+      </c>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="15">
+        <f>E29+F30</f>
+        <v>400</v>
+      </c>
+      <c r="F30" s="7">
+        <v>-200</v>
+      </c>
+      <c r="G30" s="7">
+        <v>6003</v>
+      </c>
+      <c r="H30" s="8">
+        <v>2</v>
+      </c>
+      <c r="I30" s="8">
+        <v>4</v>
+      </c>
+      <c r="J30" s="8">
+        <v>2</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" s="8">
+        <v>2</v>
+      </c>
+      <c r="M30" s="8">
         <v>5</v>
       </c>
-      <c r="N29" s="2"/>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="10" t="s">
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="16">
-        <f t="shared" ref="E30:E33" si="2">E29+F30</f>
+      <c r="E31" s="16">
+        <f t="shared" ref="E31:E34" si="2">E30+F31</f>
         <v>395</v>
       </c>
-      <c r="F30" s="10">
-        <f>-F28*$G$8</f>
+      <c r="F31" s="10">
+        <f>-F29*$G$8</f>
         <v>-5</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G31" s="10">
         <v>6002</v>
       </c>
-      <c r="H30" s="9">
-        <v>1</v>
-      </c>
-      <c r="I30" s="9">
-        <v>0</v>
-      </c>
-      <c r="J30" s="9">
+      <c r="H31" s="9">
+        <v>1</v>
+      </c>
+      <c r="I31" s="9">
+        <v>0</v>
+      </c>
+      <c r="J31" s="9">
         <v>2</v>
       </c>
-      <c r="K30" s="10" t="s">
+      <c r="K31" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="L30" s="9">
-        <v>3</v>
-      </c>
-      <c r="M30" s="4">
-        <v>0</v>
-      </c>
-      <c r="N30" s="2"/>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="E31">
+      <c r="L31" s="9">
+        <v>3</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0</v>
+      </c>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="E32">
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-      <c r="F31" s="10">
-        <f>-(F29+F27)*$G$8</f>
+      <c r="F32" s="10">
+        <f>-(F30+F28)*$G$8</f>
         <v>-15</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G32" s="10">
         <v>6002</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H32" s="9">
         <v>2</v>
       </c>
-      <c r="I31" s="9">
-        <v>0</v>
-      </c>
-      <c r="J31" s="9">
+      <c r="I32" s="9">
+        <v>0</v>
+      </c>
+      <c r="J32" s="9">
         <v>2</v>
       </c>
-      <c r="K31" s="10" t="s">
+      <c r="K32" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="L31" s="9">
-        <v>3</v>
-      </c>
-      <c r="M31" s="4">
-        <v>0</v>
-      </c>
-      <c r="N31" s="2"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="7" t="s">
+      <c r="L32" s="9">
+        <v>3</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E33" s="29">
         <f t="shared" si="2"/>
         <v>285</v>
       </c>
-      <c r="F32" s="7">
-        <f>-(F30+F28)</f>
+      <c r="F33" s="7">
+        <f>-(F31+F29)</f>
         <v>-95</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G33" s="7">
         <v>6003</v>
       </c>
-      <c r="H32" s="8">
-        <v>1</v>
-      </c>
-      <c r="I32" s="8">
+      <c r="H33" s="8">
+        <v>1</v>
+      </c>
+      <c r="I33" s="8">
         <v>2</v>
       </c>
-      <c r="J32" s="8">
+      <c r="J33" s="8">
         <v>2</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="K33" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L32" s="8">
+      <c r="L33" s="8">
         <v>4</v>
       </c>
-      <c r="M32" s="18">
+      <c r="M33" s="18">
         <v>6</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="15">
+    <row r="34" spans="1:14">
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="15">
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="F33" s="7">
-        <f>-(250+F32)</f>
+      <c r="F34" s="7">
+        <f>-(250+F33)</f>
         <v>-155</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G34" s="7">
         <v>6003</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H34" s="8">
         <v>2</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I34" s="8">
         <v>2</v>
       </c>
-      <c r="J33" s="8">
+      <c r="J34" s="8">
         <v>2</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="K34" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L33" s="8">
+      <c r="L34" s="8">
         <v>4</v>
       </c>
-      <c r="M33" s="18">
+      <c r="M34" s="18">
         <v>6</v>
       </c>
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+      <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="20" t="s">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B36" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C36" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20">
+      <c r="D36" s="20"/>
+      <c r="E36" s="20">
         <v>500</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F36" s="20">
         <v>500</v>
       </c>
-      <c r="G35" s="20">
+      <c r="G36" s="20">
         <v>6001</v>
       </c>
-      <c r="H35" s="23">
-        <v>3</v>
-      </c>
-      <c r="I35" s="23">
-        <v>0</v>
-      </c>
-      <c r="J35" s="23">
-        <v>3</v>
-      </c>
-      <c r="K35" s="20" t="s">
+      <c r="H36" s="23">
+        <v>3</v>
+      </c>
+      <c r="I36" s="23">
+        <v>0</v>
+      </c>
+      <c r="J36" s="23">
+        <v>3</v>
+      </c>
+      <c r="K36" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L35" s="23">
-        <v>1</v>
-      </c>
-      <c r="M35" s="24">
-        <v>0</v>
-      </c>
-      <c r="N35" s="2"/>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="7" t="s">
+      <c r="L36" s="23">
+        <v>1</v>
+      </c>
+      <c r="M36" s="24">
+        <v>0</v>
+      </c>
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7" t="s">
+      <c r="B37" s="8"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="7">
-        <f t="shared" ref="E36:E41" si="3">E35+F36</f>
+      <c r="E37" s="7">
+        <f t="shared" ref="E37:E42" si="3">E36+F37</f>
         <v>550</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F37" s="7">
         <v>50</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G37" s="7">
         <v>6004</v>
       </c>
-      <c r="H36" s="8">
-        <v>1</v>
-      </c>
-      <c r="I36" s="8">
-        <v>1</v>
-      </c>
-      <c r="J36" s="8">
-        <v>3</v>
-      </c>
-      <c r="K36" s="7" t="s">
+      <c r="H37" s="8">
+        <v>1</v>
+      </c>
+      <c r="I37" s="8">
+        <v>1</v>
+      </c>
+      <c r="J37" s="8">
+        <v>3</v>
+      </c>
+      <c r="K37" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="L36" s="8">
+      <c r="L37" s="8">
         <v>2</v>
       </c>
-      <c r="M36" s="8">
-        <v>3</v>
-      </c>
-      <c r="N36" s="2"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="5">
-        <f t="shared" si="3"/>
-        <v>500</v>
-      </c>
-      <c r="F37" s="5">
-        <v>-50</v>
-      </c>
-      <c r="G37" s="5">
-        <v>6003</v>
-      </c>
-      <c r="H37" s="6">
-        <v>1</v>
-      </c>
-      <c r="I37" s="6">
-        <v>1</v>
-      </c>
-      <c r="J37" s="6">
-        <v>3</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L37" s="6">
-        <v>2</v>
-      </c>
-      <c r="M37" s="6">
-        <v>4</v>
+      <c r="M37" s="8">
+        <v>3</v>
       </c>
       <c r="N37" s="2"/>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="7"/>
       <c r="B38" s="8"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="14">
+      <c r="C38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="F38" s="5">
+        <v>-50</v>
+      </c>
+      <c r="G38" s="5">
+        <v>6003</v>
+      </c>
+      <c r="H38" s="6">
+        <v>1</v>
+      </c>
+      <c r="I38" s="6">
+        <v>1</v>
+      </c>
+      <c r="J38" s="6">
+        <v>3</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L38" s="6">
+        <v>2</v>
+      </c>
+      <c r="M38" s="6">
+        <v>4</v>
+      </c>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="14">
         <f t="shared" si="3"/>
         <v>475</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F39" s="5">
         <v>-25</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G39" s="5">
         <v>6003</v>
       </c>
-      <c r="H38" s="6">
-        <v>3</v>
-      </c>
-      <c r="I38" s="6">
-        <v>1</v>
-      </c>
-      <c r="J38" s="6">
-        <v>3</v>
-      </c>
-      <c r="K38" s="5" t="s">
+      <c r="H39" s="6">
+        <v>3</v>
+      </c>
+      <c r="I39" s="6">
+        <v>1</v>
+      </c>
+      <c r="J39" s="6">
+        <v>3</v>
+      </c>
+      <c r="K39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="L38" s="6">
+      <c r="L39" s="6">
         <v>2</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M39" s="6">
         <v>4</v>
       </c>
-      <c r="N38" s="2"/>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39" s="10" t="s">
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39">
+      <c r="D40" s="10"/>
+      <c r="E40">
         <f t="shared" si="3"/>
         <v>451.25</v>
       </c>
-      <c r="F39" s="10">
-        <f>-(F38+F35)*$G$8</f>
+      <c r="F40" s="10">
+        <f>-(F39+F36)*$G$8</f>
         <v>-23.75</v>
       </c>
-      <c r="G39" s="10">
+      <c r="G40" s="10">
         <v>6002</v>
       </c>
-      <c r="H39" s="9">
-        <v>3</v>
-      </c>
-      <c r="I39" s="9">
-        <v>0</v>
-      </c>
-      <c r="J39" s="9">
-        <v>3</v>
-      </c>
-      <c r="K39" s="10" t="s">
+      <c r="H40" s="9">
+        <v>3</v>
+      </c>
+      <c r="I40" s="9">
+        <v>0</v>
+      </c>
+      <c r="J40" s="9">
+        <v>3</v>
+      </c>
+      <c r="K40" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L39" s="9">
-        <v>3</v>
-      </c>
-      <c r="M39" s="4">
-        <v>0</v>
-      </c>
-      <c r="N39" s="2"/>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="27">
+      <c r="L40" s="9">
+        <v>3</v>
+      </c>
+      <c r="M40" s="4">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="27">
         <f t="shared" si="3"/>
         <v>451.25</v>
       </c>
-      <c r="F40" s="10">
-        <f>-(F37+F36)*$G$8</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="10">
+      <c r="F41" s="10">
+        <f>-(F38+F37)*$G$8</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="10">
         <v>6002</v>
       </c>
-      <c r="H40" s="9">
-        <v>3</v>
-      </c>
-      <c r="I40" s="9">
-        <v>0</v>
-      </c>
-      <c r="J40" s="9">
-        <v>3</v>
-      </c>
-      <c r="K40" s="10" t="s">
+      <c r="H41" s="9">
+        <v>3</v>
+      </c>
+      <c r="I41" s="9">
+        <v>0</v>
+      </c>
+      <c r="J41" s="9">
+        <v>3</v>
+      </c>
+      <c r="K41" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="L40" s="9">
-        <v>3</v>
-      </c>
-      <c r="M40" s="17">
-        <v>0</v>
-      </c>
-      <c r="N40" s="1" t="s">
+      <c r="L41" s="9">
+        <v>3</v>
+      </c>
+      <c r="M41" s="17">
+        <v>0</v>
+      </c>
+      <c r="N41" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:14">
+      <c r="A42" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="5" t="s">
+      <c r="B42" s="8"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E41" s="28">
+      <c r="E42" s="28">
         <f t="shared" si="3"/>
         <v>475</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F42" s="5">
         <v>23.75</v>
-      </c>
-      <c r="G41" s="5">
-        <v>7001</v>
-      </c>
-      <c r="H41" s="6">
-        <v>3</v>
-      </c>
-      <c r="I41" s="6">
-        <v>1</v>
-      </c>
-      <c r="J41" s="6">
-        <v>3</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L41" s="6">
-        <v>4</v>
-      </c>
-      <c r="M41" s="26">
-        <v>6</v>
-      </c>
-      <c r="N41" s="2"/>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42" s="7"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="28">
-        <f t="shared" ref="E42:E43" si="4">E41+F42</f>
-        <v>701.25</v>
-      </c>
-      <c r="F42" s="5">
-        <v>226.25</v>
       </c>
       <c r="G42" s="5">
         <v>7001</v>
       </c>
       <c r="H42" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I42" s="6">
         <v>1</v>
@@ -2189,175 +2319,178 @@
       <c r="B43" s="8"/>
       <c r="C43" s="7"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="14">
+      <c r="E43" s="28">
+        <f t="shared" ref="E43:E44" si="4">E42+F43</f>
+        <v>701.25</v>
+      </c>
+      <c r="F43" s="5">
+        <v>226.25</v>
+      </c>
+      <c r="G43" s="5">
+        <v>7001</v>
+      </c>
+      <c r="H43" s="6">
+        <v>1</v>
+      </c>
+      <c r="I43" s="6">
+        <v>1</v>
+      </c>
+      <c r="J43" s="6">
+        <v>3</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L43" s="6">
+        <v>4</v>
+      </c>
+      <c r="M43" s="26">
+        <v>6</v>
+      </c>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="14">
         <f t="shared" si="4"/>
         <v>451.25</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F44" s="5">
         <v>-250</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G44" s="5">
         <v>7002</v>
       </c>
-      <c r="H43" s="6">
-        <v>3</v>
-      </c>
-      <c r="I43" s="6">
-        <v>3</v>
-      </c>
-      <c r="J43" s="6">
+      <c r="H44" s="6">
+        <v>3</v>
+      </c>
+      <c r="I44" s="6">
+        <v>3</v>
+      </c>
+      <c r="J44" s="6">
         <v>5</v>
       </c>
-      <c r="K43" s="5" t="s">
+      <c r="K44" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="L43" s="6">
+      <c r="L44" s="6">
         <v>4</v>
       </c>
-      <c r="M43" s="26">
+      <c r="M44" s="26">
         <v>6</v>
       </c>
-      <c r="N43" s="2"/>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="20" t="s">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B46" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C46" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20">
+      <c r="D46" s="20"/>
+      <c r="E46" s="20">
         <v>500</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F46" s="20">
         <v>500</v>
       </c>
-      <c r="G45" s="20">
+      <c r="G46" s="20">
         <v>6001</v>
       </c>
-      <c r="H45" s="23">
+      <c r="H46" s="23">
         <v>4</v>
       </c>
-      <c r="I45" s="23">
-        <v>0</v>
-      </c>
-      <c r="J45" s="23">
+      <c r="I46" s="23">
+        <v>0</v>
+      </c>
+      <c r="J46" s="23">
         <v>4</v>
       </c>
-      <c r="K45" s="20" t="s">
+      <c r="K46" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L45" s="23">
-        <v>1</v>
-      </c>
-      <c r="M45" s="24">
-        <v>0</v>
-      </c>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="A46" s="7" t="s">
+      <c r="L46" s="23">
+        <v>1</v>
+      </c>
+      <c r="M46" s="24">
+        <v>0</v>
+      </c>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7" t="s">
+      <c r="B47" s="8"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="15">
-        <f>E45+F46</f>
+      <c r="E47" s="15">
+        <f>E46+F47</f>
         <v>700</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F47" s="7">
         <v>200</v>
       </c>
-      <c r="G46" s="7">
+      <c r="G47" s="7">
         <v>6004</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H47" s="8">
         <v>2</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I47" s="8">
         <v>2</v>
       </c>
-      <c r="J46" s="8">
+      <c r="J47" s="8">
         <v>4</v>
       </c>
-      <c r="K46" s="7" t="s">
+      <c r="K47" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L46" s="8">
+      <c r="L47" s="8">
         <v>2</v>
       </c>
-      <c r="M46" s="8">
+      <c r="M47" s="8">
         <v>5</v>
       </c>
-      <c r="N46" s="2"/>
-    </row>
-    <row r="47" spans="1:14">
-      <c r="A47" s="10" t="s">
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10">
-        <f>E46+F47</f>
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10">
+        <f>E47+F48</f>
         <v>690</v>
       </c>
-      <c r="F47" s="10">
-        <f>-F46*$G$8</f>
+      <c r="F48" s="10">
+        <f>-F47*$G$8</f>
         <v>-10</v>
-      </c>
-      <c r="G47" s="10">
-        <v>6002</v>
-      </c>
-      <c r="H47" s="9">
-        <v>2</v>
-      </c>
-      <c r="I47" s="9">
-        <v>0</v>
-      </c>
-      <c r="J47" s="9">
-        <v>4</v>
-      </c>
-      <c r="K47" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="L47" s="9">
-        <v>3</v>
-      </c>
-      <c r="M47" s="17">
-        <v>0</v>
-      </c>
-      <c r="N47" s="2"/>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="E48" s="16">
-        <f>E47+F48</f>
-        <v>665</v>
-      </c>
-      <c r="F48" s="10">
-        <f>-F45*$G$8</f>
-        <v>-25</v>
       </c>
       <c r="G48" s="10">
         <v>6002</v>
       </c>
       <c r="H48" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I48" s="9">
         <v>0</v>
@@ -2366,368 +2499,365 @@
         <v>4</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L48" s="9">
         <v>3</v>
       </c>
-      <c r="M48" s="4">
+      <c r="M48" s="17">
         <v>0</v>
       </c>
       <c r="N48" s="2"/>
     </row>
     <row r="49" spans="1:14">
-      <c r="A49" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="29">
+      <c r="E49" s="16">
         <f>E48+F49</f>
         <v>665</v>
       </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="12"/>
+      <c r="F49" s="10">
+        <f>-F46*$G$8</f>
+        <v>-25</v>
+      </c>
+      <c r="G49" s="10">
+        <v>6002</v>
+      </c>
+      <c r="H49" s="9">
+        <v>4</v>
+      </c>
+      <c r="I49" s="9">
+        <v>0</v>
+      </c>
+      <c r="J49" s="9">
+        <v>4</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L49" s="9">
+        <v>3</v>
+      </c>
+      <c r="M49" s="4">
+        <v>0</v>
+      </c>
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14">
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
+      <c r="A50" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="29">
+        <f>E49+F50</f>
+        <v>665</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="12"/>
       <c r="N50" s="2"/>
     </row>
     <row r="51" spans="1:14">
-      <c r="A51" s="20" t="s">
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B52" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C52" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="22">
+      <c r="D52" s="20"/>
+      <c r="E52" s="22">
         <v>500</v>
       </c>
-      <c r="F51" s="20">
+      <c r="F52" s="20">
         <v>500</v>
       </c>
-      <c r="G51" s="20">
+      <c r="G52" s="20">
         <v>6001</v>
       </c>
-      <c r="H51" s="23">
+      <c r="H52" s="23">
         <v>5</v>
       </c>
-      <c r="I51" s="23">
-        <v>0</v>
-      </c>
-      <c r="J51" s="23">
+      <c r="I52" s="23">
+        <v>0</v>
+      </c>
+      <c r="J52" s="23">
         <v>5</v>
       </c>
-      <c r="K51" s="20" t="s">
+      <c r="K52" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L51" s="23">
-        <v>1</v>
-      </c>
-      <c r="M51" s="24">
-        <v>0</v>
-      </c>
-      <c r="N51" s="2"/>
-    </row>
-    <row r="52" spans="1:14">
-      <c r="A52" s="7" t="s">
+      <c r="L52" s="23">
+        <v>1</v>
+      </c>
+      <c r="M52" s="24">
+        <v>0</v>
+      </c>
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="13">
-        <f>E51+F52</f>
+      <c r="B53" s="8"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="13">
+        <f>E52+F53</f>
         <v>500</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="2"/>
-    </row>
-    <row r="53" spans="1:14">
-      <c r="A53" s="10" t="s">
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="16">
-        <f>E51+F53</f>
+      <c r="E54" s="16">
+        <f>E52+F54</f>
         <v>475</v>
       </c>
-      <c r="F53">
-        <f>-F51*$G$8</f>
+      <c r="F54">
+        <f>-F52*$G$8</f>
         <v>-25</v>
       </c>
-      <c r="G53">
+      <c r="G54">
         <v>6002</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H54" s="2">
         <v>5</v>
       </c>
-      <c r="I53" s="2">
-        <v>0</v>
-      </c>
-      <c r="J53" s="2">
+      <c r="I54" s="2">
+        <v>0</v>
+      </c>
+      <c r="J54" s="2">
         <v>5</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K54" t="s">
         <v>62</v>
       </c>
-      <c r="L53" s="2">
-        <v>3</v>
-      </c>
-      <c r="M53" s="4">
-        <v>0</v>
-      </c>
-      <c r="N53" s="2"/>
-    </row>
-    <row r="54" spans="1:14">
-      <c r="A54" s="7" t="s">
+      <c r="L54" s="2">
+        <v>3</v>
+      </c>
+      <c r="M54" s="4">
+        <v>0</v>
+      </c>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="15">
-        <f>E53+F54</f>
+      <c r="B55" s="8"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="15">
+        <f>E54+F55</f>
         <v>725</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F55" s="7">
         <v>250</v>
       </c>
-      <c r="G54" s="7">
+      <c r="G55" s="7">
         <v>6002</v>
       </c>
-      <c r="H54" s="8">
-        <v>3</v>
-      </c>
-      <c r="I54" s="8">
-        <v>3</v>
-      </c>
-      <c r="J54" s="8">
+      <c r="H55" s="8">
+        <v>3</v>
+      </c>
+      <c r="I55" s="8">
+        <v>3</v>
+      </c>
+      <c r="J55" s="8">
         <v>5</v>
       </c>
-      <c r="K54" s="7" t="s">
+      <c r="K55" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L54" s="8">
+      <c r="L55" s="8">
         <v>4</v>
       </c>
-      <c r="M54" s="18">
+      <c r="M55" s="18">
         <v>6</v>
       </c>
-      <c r="N54" s="2"/>
-    </row>
-    <row r="55" spans="1:14">
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
       <c r="N55" s="2"/>
     </row>
     <row r="56" spans="1:14">
-      <c r="A56" s="20" t="s">
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B57" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C57" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="22">
+      <c r="D57" s="20"/>
+      <c r="E57" s="22">
         <v>500</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F57" s="20">
         <v>500</v>
       </c>
-      <c r="G56" s="20">
+      <c r="G57" s="20">
         <v>6001</v>
       </c>
-      <c r="H56" s="23">
+      <c r="H57" s="23">
         <v>6</v>
       </c>
-      <c r="I56" s="23">
-        <v>0</v>
-      </c>
-      <c r="J56" s="23">
+      <c r="I57" s="23">
+        <v>0</v>
+      </c>
+      <c r="J57" s="23">
         <v>6</v>
       </c>
-      <c r="K56" s="20" t="s">
+      <c r="K57" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L56" s="23">
-        <v>1</v>
-      </c>
-      <c r="M56" s="24">
-        <v>0</v>
-      </c>
-      <c r="N56" s="2"/>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57" s="7" t="s">
+      <c r="L57" s="23">
+        <v>1</v>
+      </c>
+      <c r="M57" s="24">
+        <v>0</v>
+      </c>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="13">
-        <f>E56+F57</f>
+      <c r="B58" s="8"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="13">
+        <f>E57+F58</f>
         <v>500</v>
       </c>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="12"/>
-      <c r="N57" s="2"/>
-    </row>
-    <row r="58" spans="1:14">
-      <c r="A58" s="10" t="s">
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="12"/>
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E58" s="16">
-        <f>E56+F58</f>
+      <c r="E59" s="16">
+        <f>E57+F59</f>
         <v>475</v>
       </c>
-      <c r="F58">
-        <f>-F56*$G$8</f>
+      <c r="F59">
+        <f>-F57*$G$8</f>
         <v>-25</v>
       </c>
-      <c r="G58">
+      <c r="G59">
         <v>6002</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H59" s="2">
         <v>6</v>
       </c>
-      <c r="I58" s="2">
-        <v>0</v>
-      </c>
-      <c r="J58" s="2">
+      <c r="I59" s="2">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2">
         <v>6</v>
       </c>
-      <c r="K58" t="s">
+      <c r="K59" t="s">
         <v>67</v>
       </c>
-      <c r="L58" s="2">
-        <v>3</v>
-      </c>
-      <c r="M58" s="4">
-        <v>0</v>
-      </c>
-      <c r="N58" s="2"/>
-    </row>
-    <row r="59" spans="1:14">
-      <c r="A59" s="7" t="s">
+      <c r="L59" s="2">
+        <v>3</v>
+      </c>
+      <c r="M59" s="4">
+        <v>0</v>
+      </c>
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="29">
-        <f>E58+F59</f>
+      <c r="B60" s="8"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="29">
+        <f>E59+F60</f>
         <v>475</v>
       </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="8"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="2"/>
-    </row>
-    <row r="60" spans="1:14">
-      <c r="A60" s="10" t="s">
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="2"/>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E60" s="28">
-        <f>E59+F60</f>
-        <v>575</v>
-      </c>
-      <c r="F60" s="5">
-        <v>100</v>
-      </c>
-      <c r="G60" s="5">
-        <v>7002</v>
-      </c>
-      <c r="H60" s="6">
-        <v>8</v>
-      </c>
-      <c r="I60" s="6">
-        <v>8</v>
-      </c>
-      <c r="J60" s="6">
-        <v>6</v>
-      </c>
-      <c r="K60" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="L60" s="6">
-        <v>5</v>
-      </c>
-      <c r="M60" s="26">
-        <v>7</v>
-      </c>
-      <c r="N60" s="2"/>
-    </row>
-    <row r="61" spans="1:14">
-      <c r="A61" s="10"/>
       <c r="B61" s="9"/>
       <c r="C61" s="10"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="14">
+      <c r="D61" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E61" s="28">
         <f>E60+F61</f>
-        <v>475</v>
+        <v>575</v>
       </c>
       <c r="F61" s="5">
-        <v>-100</v>
+        <v>100</v>
       </c>
       <c r="G61" s="5">
-        <v>7001</v>
+        <v>7002</v>
       </c>
       <c r="H61" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I61" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J61" s="6">
         <v>6</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L61" s="6">
         <v>5</v>
@@ -2738,188 +2868,228 @@
       <c r="N61" s="2"/>
     </row>
     <row r="62" spans="1:14">
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="14">
+        <f>E61+F62</f>
+        <v>475</v>
+      </c>
+      <c r="F62" s="5">
+        <v>-100</v>
+      </c>
+      <c r="G62" s="5">
+        <v>7001</v>
+      </c>
+      <c r="H62" s="6">
+        <v>6</v>
+      </c>
+      <c r="I62" s="6">
+        <v>1</v>
+      </c>
+      <c r="J62" s="6">
+        <v>6</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="L62" s="6">
+        <v>5</v>
+      </c>
+      <c r="M62" s="26">
+        <v>7</v>
+      </c>
       <c r="N62" s="2"/>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="22">
-        <v>500</v>
-      </c>
-      <c r="F63" s="20">
-        <v>500</v>
-      </c>
-      <c r="G63" s="20">
-        <v>6001</v>
-      </c>
-      <c r="H63" s="23">
-        <v>7</v>
-      </c>
-      <c r="I63" s="23">
-        <v>0</v>
-      </c>
-      <c r="J63" s="23">
-        <v>7</v>
-      </c>
-      <c r="K63" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="L63" s="23">
-        <v>1</v>
-      </c>
-      <c r="M63" s="24">
-        <v>0</v>
+      <c r="A63" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63" s="28">
+        <f>E62+F63</f>
+        <v>600</v>
+      </c>
+      <c r="F63" s="5">
+        <v>125</v>
+      </c>
+      <c r="G63" s="5">
+        <v>7002</v>
+      </c>
+      <c r="H63" s="6">
+        <v>8</v>
+      </c>
+      <c r="I63" s="6">
+        <v>8</v>
+      </c>
+      <c r="J63" s="6">
+        <v>6</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L63" s="6">
+        <v>6</v>
+      </c>
+      <c r="M63" s="26">
+        <v>8</v>
       </c>
       <c r="N63" s="2"/>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="A64" s="7"/>
       <c r="B64" s="8"/>
       <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="13">
+      <c r="D64" s="5"/>
+      <c r="E64" s="14">
         <f>E63+F64</f>
+        <v>475</v>
+      </c>
+      <c r="F64" s="5">
+        <v>-125</v>
+      </c>
+      <c r="G64" s="5">
+        <v>7001</v>
+      </c>
+      <c r="H64" s="6">
+        <v>6</v>
+      </c>
+      <c r="I64" s="6">
+        <v>1</v>
+      </c>
+      <c r="J64" s="6">
+        <v>6</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="L64" s="6">
+        <v>6</v>
+      </c>
+      <c r="M64" s="26">
+        <v>8</v>
+      </c>
+      <c r="N64" s="2"/>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" s="20"/>
+      <c r="E66" s="22">
         <v>500</v>
       </c>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="12"/>
-      <c r="N64" s="2"/>
-    </row>
-    <row r="65" spans="1:14">
-      <c r="A65" s="10" t="s">
+      <c r="F66" s="20">
+        <v>500</v>
+      </c>
+      <c r="G66" s="20">
+        <v>6001</v>
+      </c>
+      <c r="H66" s="23">
+        <v>7</v>
+      </c>
+      <c r="I66" s="23">
+        <v>0</v>
+      </c>
+      <c r="J66" s="23">
+        <v>7</v>
+      </c>
+      <c r="K66" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L66" s="23">
+        <v>1</v>
+      </c>
+      <c r="M66" s="24">
+        <v>0</v>
+      </c>
+      <c r="N66" s="2"/>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="13">
+        <f>E66+F67</f>
+        <v>500</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="8"/>
+      <c r="M67" s="12"/>
+      <c r="N67" s="2"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E65" s="16">
-        <f>E63+F65</f>
+      <c r="E68" s="16">
+        <f>E66+F68</f>
         <v>475</v>
       </c>
-      <c r="F65">
-        <f>-F63*$G$8</f>
+      <c r="F68">
+        <f>-F66*$G$8</f>
         <v>-25</v>
       </c>
-      <c r="G65">
+      <c r="G68">
         <v>6002</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H68" s="2">
         <v>7</v>
       </c>
-      <c r="I65" s="2">
-        <v>0</v>
-      </c>
-      <c r="J65" s="2">
+      <c r="I68" s="2">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2">
         <v>7</v>
       </c>
-      <c r="K65" t="s">
+      <c r="K68" t="s">
         <v>66</v>
       </c>
-      <c r="L65" s="2">
-        <v>3</v>
-      </c>
-      <c r="M65" s="4">
-        <v>0</v>
-      </c>
-      <c r="N65" s="2"/>
-    </row>
-    <row r="66" spans="1:14">
-      <c r="A66" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="29">
-        <f>E65+F66</f>
-        <v>475</v>
-      </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="12"/>
-      <c r="N66" s="2"/>
-    </row>
-    <row r="67" spans="1:14">
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-    </row>
-    <row r="68" spans="1:14">
-      <c r="A68" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="20"/>
-      <c r="E68" s="22">
-        <v>500</v>
-      </c>
-      <c r="F68" s="20">
-        <v>500</v>
-      </c>
-      <c r="G68" s="20">
-        <v>6001</v>
-      </c>
-      <c r="H68" s="23">
-        <v>8</v>
-      </c>
-      <c r="I68" s="23">
-        <v>0</v>
-      </c>
-      <c r="J68" s="23">
-        <v>8</v>
-      </c>
-      <c r="K68" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="L68" s="23">
-        <v>1</v>
-      </c>
-      <c r="M68" s="24">
+      <c r="L68" s="2">
+        <v>3</v>
+      </c>
+      <c r="M68" s="4">
         <v>0</v>
       </c>
       <c r="N68" s="2"/>
     </row>
     <row r="69" spans="1:14">
       <c r="A69" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="13">
+      <c r="E69" s="29">
         <f>E68+F69</f>
-        <v>500</v>
+        <v>475</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
@@ -2932,223 +3102,241 @@
       <c r="N69" s="2"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="10" t="s">
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" s="20"/>
+      <c r="E71" s="22">
+        <v>500</v>
+      </c>
+      <c r="F71" s="20">
+        <v>500</v>
+      </c>
+      <c r="G71" s="20">
+        <v>6001</v>
+      </c>
+      <c r="H71" s="23">
+        <v>8</v>
+      </c>
+      <c r="I71" s="23">
+        <v>0</v>
+      </c>
+      <c r="J71" s="23">
+        <v>8</v>
+      </c>
+      <c r="K71" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L71" s="23">
+        <v>1</v>
+      </c>
+      <c r="M71" s="24">
+        <v>0</v>
+      </c>
+      <c r="N71" s="2"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="13">
+        <f>E71+F72</f>
+        <v>500</v>
+      </c>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="12"/>
+      <c r="N72" s="2"/>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E70" s="16">
-        <f>E68+F70</f>
+      <c r="E73" s="16">
+        <f>E71+F73</f>
         <v>475</v>
       </c>
-      <c r="F70">
-        <f>-F68*$G$8</f>
+      <c r="F73">
+        <f>-F71*$G$8</f>
         <v>-25</v>
       </c>
-      <c r="G70">
+      <c r="G73">
         <v>6002</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H73" s="2">
         <v>8</v>
       </c>
-      <c r="I70" s="2">
-        <v>0</v>
-      </c>
-      <c r="J70" s="2">
+      <c r="I73" s="2">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2">
         <v>8</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K73" t="s">
         <v>65</v>
       </c>
-      <c r="L70" s="2">
-        <v>3</v>
-      </c>
-      <c r="M70" s="4">
-        <v>0</v>
-      </c>
-      <c r="N70" s="2"/>
-    </row>
-    <row r="71" spans="1:14">
-      <c r="A71" s="7" t="s">
+      <c r="L73" s="2">
+        <v>3</v>
+      </c>
+      <c r="M73" s="4">
+        <v>0</v>
+      </c>
+      <c r="N73" s="2"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="8"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="29">
-        <f>E70+F71</f>
+      <c r="B74" s="8"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="29">
+        <f>E73+F74</f>
         <v>475</v>
       </c>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="8"/>
-      <c r="M71" s="12"/>
-      <c r="N71" s="2"/>
-    </row>
-    <row r="72" spans="1:14">
-      <c r="A72" s="10" t="s">
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="8"/>
+      <c r="M74" s="12"/>
+      <c r="N74" s="2"/>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10" t="s">
+      <c r="B75" s="9"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E72" s="27">
-        <f>E71+F72</f>
+      <c r="E75" s="27">
+        <f>E74+F75</f>
         <v>375</v>
       </c>
-      <c r="F72" s="10">
+      <c r="F75" s="10">
         <v>-100</v>
       </c>
-      <c r="G72" s="10">
+      <c r="G75" s="10">
         <v>6003</v>
       </c>
-      <c r="H72" s="9">
+      <c r="H75" s="9">
         <v>8</v>
       </c>
-      <c r="I72" s="9">
+      <c r="I75" s="9">
         <v>6</v>
       </c>
-      <c r="J72" s="9">
+      <c r="J75" s="9">
         <v>8</v>
       </c>
-      <c r="K72" s="10" t="s">
+      <c r="K75" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="L72" s="9">
+      <c r="L75" s="9">
         <v>5</v>
       </c>
-      <c r="M72" s="25">
+      <c r="M75" s="25">
         <v>7</v>
       </c>
-      <c r="N72" s="2"/>
-    </row>
-    <row r="73" spans="1:14">
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
-    </row>
-    <row r="74" spans="1:14">
-      <c r="A74" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B74" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D74" s="20"/>
-      <c r="E74" s="22">
+      <c r="N75" s="2"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E76" s="28">
+        <f>E75+F76</f>
         <v>500</v>
       </c>
-      <c r="F74" s="20">
-        <v>500</v>
-      </c>
-      <c r="G74" s="20">
-        <v>6001</v>
-      </c>
-      <c r="H74" s="23">
+      <c r="F76" s="5">
+        <v>125</v>
+      </c>
+      <c r="G76" s="5">
+        <v>7002</v>
+      </c>
+      <c r="H76" s="6">
         <v>9</v>
       </c>
-      <c r="I74" s="23">
-        <v>0</v>
-      </c>
-      <c r="J74" s="23">
+      <c r="I76" s="6">
         <v>9</v>
       </c>
-      <c r="K74" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="L74" s="23">
-        <v>1</v>
-      </c>
-      <c r="M74" s="24">
-        <v>0</v>
-      </c>
-      <c r="N74" s="2"/>
-    </row>
-    <row r="75" spans="1:14">
-      <c r="A75" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="13">
-        <f>E74+F75</f>
-        <v>500</v>
-      </c>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="7"/>
-      <c r="L75" s="8"/>
-      <c r="M75" s="12"/>
-      <c r="N75" s="2"/>
-    </row>
-    <row r="76" spans="1:14">
-      <c r="A76" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E76" s="16">
-        <f>E74+F76</f>
-        <v>475</v>
-      </c>
-      <c r="F76">
-        <f>-F74*$G$8</f>
-        <v>-25</v>
-      </c>
-      <c r="G76">
-        <v>6002</v>
-      </c>
-      <c r="H76" s="2">
-        <v>9</v>
-      </c>
-      <c r="I76" s="2">
-        <v>0</v>
-      </c>
-      <c r="J76" s="2">
-        <v>9</v>
-      </c>
-      <c r="K76" t="s">
-        <v>64</v>
-      </c>
-      <c r="L76" s="2">
-        <v>3</v>
-      </c>
-      <c r="M76" s="4">
-        <v>0</v>
+      <c r="J76" s="6">
+        <v>8</v>
+      </c>
+      <c r="K76" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="L76" s="6">
+        <v>6</v>
+      </c>
+      <c r="M76" s="26">
+        <v>8</v>
       </c>
       <c r="N76" s="2"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="A77" s="7"/>
       <c r="B77" s="8"/>
       <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="29">
+      <c r="D77" s="5"/>
+      <c r="E77" s="14">
         <f>E76+F77</f>
-        <v>475</v>
-      </c>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
-      <c r="J77" s="8"/>
-      <c r="K77" s="7"/>
-      <c r="L77" s="8"/>
-      <c r="M77" s="12"/>
+        <v>375</v>
+      </c>
+      <c r="F77" s="5">
+        <v>-125</v>
+      </c>
+      <c r="G77" s="5">
+        <v>7001</v>
+      </c>
+      <c r="H77" s="6">
+        <v>8</v>
+      </c>
+      <c r="I77" s="6">
+        <v>6</v>
+      </c>
+      <c r="J77" s="6">
+        <v>8</v>
+      </c>
+      <c r="K77" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="L77" s="6">
+        <v>6</v>
+      </c>
+      <c r="M77" s="26">
+        <v>8</v>
+      </c>
       <c r="N77" s="2"/>
     </row>
     <row r="78" spans="1:14">
@@ -3164,10 +3352,10 @@
         <v>68</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D79" s="20"/>
       <c r="E79" s="22">
@@ -3180,13 +3368,13 @@
         <v>6001</v>
       </c>
       <c r="H79" s="23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I79" s="23">
         <v>0</v>
       </c>
       <c r="J79" s="23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K79" s="20" t="s">
         <v>13</v>
@@ -3236,16 +3424,16 @@
         <v>6002</v>
       </c>
       <c r="H81" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I81" s="2">
         <v>0</v>
       </c>
       <c r="J81" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K81" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L81" s="2">
         <v>3</v>
@@ -3277,19 +3465,77 @@
       <c r="N82" s="2"/>
     </row>
     <row r="83" spans="1:14">
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
-      <c r="L83" s="2"/>
-      <c r="M83" s="2"/>
+      <c r="A83" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="9"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E83" s="28">
+        <f>E82+F83</f>
+        <v>600</v>
+      </c>
+      <c r="F83" s="5">
+        <v>125</v>
+      </c>
+      <c r="G83" s="5">
+        <v>7002</v>
+      </c>
+      <c r="H83" s="6">
+        <v>10</v>
+      </c>
+      <c r="I83" s="6">
+        <v>10</v>
+      </c>
+      <c r="J83" s="6">
+        <v>9</v>
+      </c>
+      <c r="K83" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="L83" s="6">
+        <v>6</v>
+      </c>
+      <c r="M83" s="26">
+        <v>8</v>
+      </c>
       <c r="N83" s="2"/>
     </row>
     <row r="84" spans="1:14">
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="14">
+        <f>E83+F84</f>
+        <v>475</v>
+      </c>
+      <c r="F84" s="5">
+        <v>-125</v>
+      </c>
+      <c r="G84" s="5">
+        <v>7001</v>
+      </c>
+      <c r="H84" s="6">
+        <v>9</v>
+      </c>
+      <c r="I84" s="6">
+        <v>8</v>
+      </c>
+      <c r="J84" s="6">
+        <v>9</v>
+      </c>
+      <c r="K84" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L84" s="6">
+        <v>6</v>
+      </c>
+      <c r="M84" s="26">
+        <v>8</v>
+      </c>
       <c r="N84" s="2"/>
     </row>
     <row r="85" spans="1:14">
@@ -3298,31 +3544,201 @@
       <c r="J85" s="2"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
     </row>
     <row r="86" spans="1:14">
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
+      <c r="A86" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D86" s="20"/>
+      <c r="E86" s="22">
+        <v>500</v>
+      </c>
+      <c r="F86" s="20">
+        <v>500</v>
+      </c>
+      <c r="G86" s="20">
+        <v>6001</v>
+      </c>
+      <c r="H86" s="23">
+        <v>10</v>
+      </c>
+      <c r="I86" s="23">
+        <v>0</v>
+      </c>
+      <c r="J86" s="23">
+        <v>10</v>
+      </c>
+      <c r="K86" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L86" s="23">
+        <v>1</v>
+      </c>
+      <c r="M86" s="24">
+        <v>0</v>
+      </c>
+      <c r="N86" s="2"/>
     </row>
     <row r="87" spans="1:14">
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
+      <c r="A87" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="8"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="13">
+        <f>E86+F87</f>
+        <v>500</v>
+      </c>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="8"/>
+      <c r="K87" s="7"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="12"/>
+      <c r="N87" s="2"/>
     </row>
     <row r="88" spans="1:14">
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
+      <c r="A88" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E88" s="16">
+        <f>E86+F88</f>
+        <v>475</v>
+      </c>
+      <c r="F88">
+        <f>-F86*$G$8</f>
+        <v>-25</v>
+      </c>
+      <c r="G88">
+        <v>6002</v>
+      </c>
+      <c r="H88" s="2">
+        <v>10</v>
+      </c>
+      <c r="I88" s="2">
+        <v>0</v>
+      </c>
+      <c r="J88" s="2">
+        <v>10</v>
+      </c>
+      <c r="K88" t="s">
+        <v>63</v>
+      </c>
+      <c r="L88" s="2">
+        <v>3</v>
+      </c>
+      <c r="M88" s="4">
+        <v>0</v>
+      </c>
+      <c r="N88" s="2"/>
     </row>
     <row r="89" spans="1:14">
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
+      <c r="A89" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B89" s="8"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="29">
+        <f>E88+F89</f>
+        <v>475</v>
+      </c>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="7"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="12"/>
+      <c r="N89" s="2"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
+      <c r="A90" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D90" t="s">
+        <v>90</v>
+      </c>
+      <c r="E90" s="16">
+        <f>E89+F90</f>
+        <v>350</v>
+      </c>
+      <c r="F90">
+        <v>-125</v>
+      </c>
+      <c r="G90">
+        <v>6004</v>
+      </c>
+      <c r="H90" s="2">
+        <v>10</v>
+      </c>
+      <c r="I90" s="2">
+        <v>9</v>
+      </c>
+      <c r="J90" s="2">
+        <v>10</v>
+      </c>
+      <c r="K90" t="s">
+        <v>91</v>
+      </c>
+      <c r="L90" s="2">
+        <v>6</v>
+      </c>
+      <c r="M90" s="2">
+        <v>8</v>
+      </c>
+      <c r="N90" s="2"/>
+    </row>
+    <row r="91" spans="1:14">
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="2"/>
+      <c r="N91" s="2"/>
+    </row>
+    <row r="92" spans="1:14">
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+    </row>
+    <row r="93" spans="1:14">
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+    </row>
+    <row r="94" spans="1:14">
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95" spans="1:14">
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+    </row>
+    <row r="96" spans="1:14">
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="8:10">
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3337,13 +3753,659 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13">
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="B6" s="2"/>
+      <c r="D6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20">
+        <v>500</v>
+      </c>
+      <c r="F8" s="20">
+        <v>500</v>
+      </c>
+      <c r="G8" s="20">
+        <v>6001</v>
+      </c>
+      <c r="H8" s="23">
+        <v>1</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0</v>
+      </c>
+      <c r="J8" s="23">
+        <v>1</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="23">
+        <v>1</v>
+      </c>
+      <c r="M8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9">
+        <f>E8+F9</f>
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>-400</v>
+      </c>
+      <c r="G9">
+        <v>6003</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>6</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" s="2">
+        <v>2</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <f>E9+F10</f>
+        <v>350</v>
+      </c>
+      <c r="F10">
+        <v>250</v>
+      </c>
+      <c r="G10">
+        <v>6004</v>
+      </c>
+      <c r="H10" s="2">
+        <v>3</v>
+      </c>
+      <c r="I10" s="2">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>104</v>
+      </c>
+      <c r="L10" s="2">
+        <v>3</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="31">
+        <f>E10+F11</f>
+        <v>101</v>
+      </c>
+      <c r="F11">
+        <v>-249</v>
+      </c>
+      <c r="G11">
+        <v>6003</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4</v>
+      </c>
+      <c r="M11" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20">
+        <v>500</v>
+      </c>
+      <c r="F13" s="20">
+        <v>500</v>
+      </c>
+      <c r="G13" s="20">
+        <v>6001</v>
+      </c>
+      <c r="H13" s="23">
+        <v>2</v>
+      </c>
+      <c r="I13" s="23">
+        <v>0</v>
+      </c>
+      <c r="J13" s="23">
+        <v>2</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="23">
+        <v>1</v>
+      </c>
+      <c r="M13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="33">
+        <f>E13+F14</f>
+        <v>749</v>
+      </c>
+      <c r="F14" s="32">
+        <v>249</v>
+      </c>
+      <c r="G14" s="32">
+        <v>6004</v>
+      </c>
+      <c r="H14" s="2">
+        <v>4</v>
+      </c>
+      <c r="I14" s="2">
+        <v>4</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+      <c r="K14" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="2">
+        <v>4</v>
+      </c>
+      <c r="M14" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20">
+        <v>500</v>
+      </c>
+      <c r="F16" s="20">
+        <v>500</v>
+      </c>
+      <c r="G16" s="20">
+        <v>6001</v>
+      </c>
+      <c r="H16" s="23">
+        <v>3</v>
+      </c>
+      <c r="I16" s="23">
+        <v>0</v>
+      </c>
+      <c r="J16" s="23">
+        <v>3</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="23">
+        <v>1</v>
+      </c>
+      <c r="M16" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17">
+        <f>E16+F17</f>
+        <v>250</v>
+      </c>
+      <c r="F17">
+        <v>-250</v>
+      </c>
+      <c r="G17">
+        <v>6003</v>
+      </c>
+      <c r="H17" s="2">
+        <v>3</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>103</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3</v>
+      </c>
+      <c r="M17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18">
+        <f>E17+F18</f>
+        <v>499</v>
+      </c>
+      <c r="F18">
+        <v>249</v>
+      </c>
+      <c r="G18">
+        <v>7001</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>79</v>
+      </c>
+      <c r="L18" s="2">
+        <v>4</v>
+      </c>
+      <c r="M18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="E19" s="31">
+        <f>E18+F19</f>
+        <v>250</v>
+      </c>
+      <c r="F19">
+        <v>-249</v>
+      </c>
+      <c r="G19">
+        <v>7002</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3</v>
+      </c>
+      <c r="I19" s="2">
+        <v>4</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
+        <v>109</v>
+      </c>
+      <c r="L19" s="2">
+        <v>4</v>
+      </c>
+      <c r="M19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20">
+        <v>500</v>
+      </c>
+      <c r="F21" s="20">
+        <v>500</v>
+      </c>
+      <c r="G21" s="20">
+        <v>6001</v>
+      </c>
+      <c r="H21" s="23">
+        <v>4</v>
+      </c>
+      <c r="I21" s="23">
+        <v>0</v>
+      </c>
+      <c r="J21" s="23">
+        <v>4</v>
+      </c>
+      <c r="K21" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="23">
+        <v>1</v>
+      </c>
+      <c r="M21" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22">
+        <f>E21+F22</f>
+        <v>749</v>
+      </c>
+      <c r="F22">
+        <v>249</v>
+      </c>
+      <c r="G22">
+        <v>7001</v>
+      </c>
+      <c r="H22" s="2">
+        <v>3</v>
+      </c>
+      <c r="I22" s="2">
+        <v>3</v>
+      </c>
+      <c r="J22" s="2">
+        <v>4</v>
+      </c>
+      <c r="K22" t="s">
+        <v>110</v>
+      </c>
+      <c r="L22" s="2">
+        <v>4</v>
+      </c>
+      <c r="M22" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="E23" s="31">
+        <f>E22+F23</f>
+        <v>500</v>
+      </c>
+      <c r="F23">
+        <v>-249</v>
+      </c>
+      <c r="G23">
+        <v>7002</v>
+      </c>
+      <c r="H23" s="2">
+        <v>4</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2</v>
+      </c>
+      <c r="J23" s="2">
+        <v>4</v>
+      </c>
+      <c r="K23" t="s">
+        <v>111</v>
+      </c>
+      <c r="L23" s="2">
+        <v>4</v>
+      </c>
+      <c r="M23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20">
+        <v>500</v>
+      </c>
+      <c r="F25" s="20">
+        <v>500</v>
+      </c>
+      <c r="G25" s="20">
+        <v>6001</v>
+      </c>
+      <c r="H25" s="23">
+        <v>6</v>
+      </c>
+      <c r="I25" s="23">
+        <v>0</v>
+      </c>
+      <c r="J25" s="23">
+        <v>6</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="23">
+        <v>1</v>
+      </c>
+      <c r="M25" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="31">
+        <f>E25+F26</f>
+        <v>900</v>
+      </c>
+      <c r="F26">
+        <v>400</v>
+      </c>
+      <c r="G26">
+        <v>6004</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <v>6</v>
+      </c>
+      <c r="K26" t="s">
+        <v>104</v>
+      </c>
+      <c r="L26" s="2">
+        <v>2</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>